<commit_message>
Added localized text table to the list of tables scripted with sexy in the carpenter test. The C++ compiles fine, with new declaration logic, improving C++ code generation. However the test script will not yet work since we have yet to implement ITableString on the side of C++. Also Notepad++ crashes when we try to complete Sys.Type.Strings.FindLeftNoCase. We also need a function StartsWith in the Sys.Type.Strings API
</commit_message>
<xml_diff>
--- a/tables/localization-text-table.xlsx
+++ b/tables/localization-text-table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB48F4B8-294B-4FC4-83A2-DD7A751B65DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10350CD4-6E5D-43EE-B9A3-E93B62F89AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>string</t>
   </si>
@@ -117,6 +117,72 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Prinzen, die nach Parteien und Freunden streben
+Ehrgeizig für Herrschaft und Herrschaft,
+Wisse, dass die Menschen in Rom, für die wir stehen
+Eine besondere Party, haben, mit gemeinsamer Stimme,
+Bei der Wahl zum römischen Kaisertum
+Auserwählter Andronicus, Beiname Pius
+Für viele gute und große Wüsten nach Rom:
+Ein edlerer Mann, ein tapferer Krieger,
+Lebt heute nicht innerhalb der Stadtmauern:
+Er wird vom Senat nach Hause geschickt
+Von müden Kriegen gegen die barbarischen Goten;
+Das mit seinen Söhnen ein Schrecken für unsere Feinde,
+Hat ein starkes Volk unterjocht, zu Waffen erzogen.
+Zehn Jahre sind seit dem ersten Unterfangen vergangen
+Diese Ursache von Rom und mit Waffen gezüchtigt
+Der Stolz unserer Feinde: fünfmal ist er zurückgekehrt
+Nach Rom blutend, seine tapferen Söhne tragend
+In Särgen vom Feld;
+Und nun endlich, beladen mit Schreckensbeute,
+Bringt den guten Andronicus nach Rom zurück,
+Der berühmte Titus, der in Waffen blüht.
+Lasst uns zu Ehren seines Namens bitten,
+Wem würdig hättest du jetzt Erfolg gehabt.
+Und rechts vom Kapitol und Senat
+Wen du vorgibst zu ehren und zu verehren,
+Dass du dich zurückziehst und deine Kraft nachlässt;
+Entlassen Sie Ihre Anhänger und, wie es Bewerber tun sollten,
+Verteidige deine Wüsten in Frieden und Demut.</t>
+  </si>
+  <si>
+    <t>Localization Table</t>
+  </si>
+  <si>
+    <t>Mark Anthony Taylor</t>
+  </si>
+  <si>
+    <t>tables\localized-text-table.h</t>
+  </si>
+  <si>
+    <t>tables\localized-text-table.cpp</t>
+  </si>
+  <si>
+    <t>ILocalizedText</t>
+  </si>
+  <si>
+    <t>LocalizedText</t>
+  </si>
+  <si>
+    <t>Rococo.Strings</t>
+  </si>
+  <si>
+    <t>Introduction_MarcusAndronicus</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>tables\rococo.tables.test.sxh</t>
+  </si>
+  <si>
+    <t>Sexy Header</t>
   </si>
   <si>
     <t>Princes, that strive by factions and by friends
@@ -147,66 +213,6 @@
 That you withdraw you and abate your strength;
 Dismiss your followers and, as suitors should,
 Plead your deserts in peace and humbleness.</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>Prinzen, die nach Parteien und Freunden streben
-Ehrgeizig für Herrschaft und Herrschaft,
-Wisse, dass die Menschen in Rom, für die wir stehen
-Eine besondere Party, haben, mit gemeinsamer Stimme,
-Bei der Wahl zum römischen Kaisertum
-Auserwählter Andronicus, Beiname Pius
-Für viele gute und große Wüsten nach Rom:
-Ein edlerer Mann, ein tapferer Krieger,
-Lebt heute nicht innerhalb der Stadtmauern:
-Er wird vom Senat nach Hause geschickt
-Von müden Kriegen gegen die barbarischen Goten;
-Das mit seinen Söhnen ein Schrecken für unsere Feinde,
-Hat ein starkes Volk unterjocht, zu Waffen erzogen.
-Zehn Jahre sind seit dem ersten Unterfangen vergangen
-Diese Ursache von Rom und mit Waffen gezüchtigt
-Der Stolz unserer Feinde: fünfmal ist er zurückgekehrt
-Nach Rom blutend, seine tapferen Söhne tragend
-In Särgen vom Feld;
-Und nun endlich, beladen mit Schreckensbeute,
-Bringt den guten Andronicus nach Rom zurück,
-Der berühmte Titus, der in Waffen blüht.
-Lasst uns zu Ehren seines Namens bitten,
-Wem würdig hättest du jetzt Erfolg gehabt.
-Und rechts vom Kapitol und Senat
-Wen du vorgibst zu ehren und zu verehren,
-Dass du dich zurückziehst und deine Kraft nachlässt;
-Entlassen Sie Ihre Anhänger und, wie es Bewerber tun sollten,
-Verteidige deine Wüsten in Frieden und Demut.</t>
-  </si>
-  <si>
-    <t>Localization Table</t>
-  </si>
-  <si>
-    <t>Mark Anthony Taylor</t>
-  </si>
-  <si>
-    <t>tables\localized-text-table.h</t>
-  </si>
-  <si>
-    <t>tables\localized-text-table.cpp</t>
-  </si>
-  <si>
-    <t>ILocalizedText</t>
-  </si>
-  <si>
-    <t>LocalizedText</t>
-  </si>
-  <si>
-    <t>Rococo.Strings</t>
-  </si>
-  <si>
-    <t>Introduction_MarcusAndronicus</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
 </sst>
 </file>
@@ -659,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -673,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -689,7 +695,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,23 +724,23 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -748,10 +754,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +781,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -783,7 +789,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -799,7 +805,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -807,7 +813,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,7 +845,15 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rococo carpenter now has the sxh definition in the config, this generally reduces the admin cost of maintaining tables, as we can eliminate the Sexy Header item from the rules in each XLSX table.
</commit_message>
<xml_diff>
--- a/tables/localization-text-table.xlsx
+++ b/tables/localization-text-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10350CD4-6E5D-43EE-B9A3-E93B62F89AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2D2170-D060-490E-8877-D8161781FC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sexcel-Spec" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>string</t>
   </si>
@@ -177,12 +177,6 @@
   </si>
   <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>tables\rococo.tables.test.sxh</t>
-  </si>
-  <si>
-    <t>Sexy Header</t>
   </si>
   <si>
     <t>Princes, that strive by factions and by friends
@@ -694,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3230684E-8A11-41FB-8526-9EA18FC7052C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -737,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>28</v>
@@ -754,10 +748,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,14 +842,6 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>